<commit_message>
MAJ Calendrier et détail des tâches
</commit_message>
<xml_diff>
--- a/Artéfacts/Artéfacts Sprint 6/Calendrier Sprint 6 - Partie 1.xlsx
+++ b/Artéfacts/Artéfacts Sprint 6/Calendrier Sprint 6 - Partie 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donoc\Desktop\L3 Informatique\Semestre 2\Projet de développement\Artéfacts\Artéfacts Sprint 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6444A0-BA97-4045-BDC5-66B9111E0DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414B9EFC-5242-4D1A-9A11-3353A9B3C116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9DAF1FEF-636C-495F-A4D9-98A6306D3E56}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>Uniformisation des balises XML avec le client</t>
   </si>
   <si>
-    <t>Ajout d'un fichier "solution" en XML</t>
-  </si>
-  <si>
     <t>Faire le tableau Excel et le détail des tâches du Sprint 6</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Tâche terminé le 02/04/2024</t>
+  </si>
+  <si>
+    <t>Ajout d'un fichier "solution" en XML pour le nouveau Corpus</t>
   </si>
 </sst>
 </file>
@@ -207,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -223,8 +223,6 @@
     <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,7 +540,7 @@
   <dimension ref="A1:AD21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +553,7 @@
       <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -573,13 +571,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -594,7 +592,7 @@
       <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="P1" s="10" t="s">
@@ -615,13 +613,13 @@
       <c r="U1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="X1" s="14" t="s">
+      <c r="V1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Y1" s="1" t="s">
@@ -636,7 +634,7 @@
       <c r="AB1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AC1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="AD1" s="12" t="s">
@@ -863,95 +861,87 @@
       <c r="C5" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="13">
-        <v>0</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
-      <c r="I5" s="13">
-        <v>0</v>
-      </c>
-      <c r="J5" s="13">
-        <v>0</v>
-      </c>
-      <c r="K5" s="13">
-        <v>0</v>
-      </c>
-      <c r="L5" s="13">
-        <v>0</v>
-      </c>
-      <c r="M5" s="13">
-        <v>0</v>
-      </c>
-      <c r="N5" s="13">
-        <v>0</v>
-      </c>
-      <c r="O5" s="13">
-        <v>0</v>
-      </c>
-      <c r="P5" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="13">
-        <v>0</v>
-      </c>
-      <c r="R5" s="13">
-        <v>0</v>
-      </c>
-      <c r="S5" s="13">
-        <v>0</v>
-      </c>
-      <c r="T5" s="13">
-        <v>0</v>
-      </c>
-      <c r="U5" s="13">
-        <v>0</v>
-      </c>
-      <c r="V5" s="13">
-        <v>0</v>
-      </c>
-      <c r="W5" s="13">
-        <v>0</v>
-      </c>
-      <c r="X5" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="13">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -961,115 +951,115 @@
         <f>B4-B5</f>
         <v>7</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7">
         <f t="shared" ref="C7:G7" si="23">B7+C4-C5</f>
         <v>6</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7">
         <f t="shared" si="23"/>
         <v>6</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7">
         <f t="shared" si="23"/>
         <v>6</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7">
         <f t="shared" si="23"/>
         <v>6</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7">
         <f t="shared" si="23"/>
         <v>6</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7">
         <f>G7+H4-H5</f>
         <v>6</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7">
         <f>H7+I4-I5</f>
         <v>6</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7">
         <f t="shared" ref="J7:AD7" si="24">I7+J4-J5</f>
         <v>6</v>
       </c>
-      <c r="K7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="L7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="M7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="N7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="O7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="P7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="Q7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="R7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="S7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="T7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="U7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="V7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="W7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="X7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="Y7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="Z7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="AA7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="AB7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="AC7" s="13">
-        <f t="shared" si="24"/>
-        <v>6</v>
-      </c>
-      <c r="AD7" s="13">
+      <c r="K7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="24"/>
+        <v>6</v>
+      </c>
+      <c r="AD7">
         <f t="shared" si="24"/>
         <v>6</v>
       </c>
@@ -1078,7 +1068,7 @@
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="Y12" s="14"/>
+      <c r="Y12" s="1"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1100,25 +1090,25 @@
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1133,7 +1123,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1176,28 +1166,25 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="13">
+        <v>27</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="13">
+        <v>23</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
     </row>
@@ -1205,7 +1192,7 @@
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12">
         <v>1</v>
       </c>
     </row>
@@ -1213,12 +1200,9 @@
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">

</xml_diff>

<commit_message>
MAJ Calendrier + détail des tâches Sprint 6
</commit_message>
<xml_diff>
--- a/Artéfacts/Artéfacts Sprint 6/Calendrier Sprint 6 - Partie 1.xlsx
+++ b/Artéfacts/Artéfacts Sprint 6/Calendrier Sprint 6 - Partie 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donoc\Desktop\L3 Informatique\Semestre 2\Projet de développement\Artéfacts\Artéfacts Sprint 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA608A6F-DA70-48B9-8788-8D7EFEBA7136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6879914B-B86E-4F27-A562-D59870189C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9DAF1FEF-636C-495F-A4D9-98A6306D3E56}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>Faire un document sur les scores de l'ensemble du Corpus</t>
   </si>
   <si>
-    <t>Faire un rapport de fin de Sprint</t>
-  </si>
-  <si>
     <t>Amélioration du code</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Tâche terminé le 09/04/2024</t>
+  </si>
+  <si>
+    <t>Faire un rapport sur l'ensemble du projet</t>
   </si>
 </sst>
 </file>
@@ -1093,25 +1093,25 @@
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1143,12 +1143,12 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>1</v>

</xml_diff>

<commit_message>
MAJ Calendrier + détail des tâches
</commit_message>
<xml_diff>
--- a/Artéfacts/Artéfacts Sprint 6/Calendrier Sprint 6 - Partie 1.xlsx
+++ b/Artéfacts/Artéfacts Sprint 6/Calendrier Sprint 6 - Partie 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donoc\Desktop\L3 Informatique\Semestre 2\Projet de développement\Artéfacts\Artéfacts Sprint 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6879914B-B86E-4F27-A562-D59870189C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91FAFB6-BF2B-47F5-A431-1409BA9C4C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9DAF1FEF-636C-495F-A4D9-98A6306D3E56}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>LUNDI</t>
   </si>
@@ -105,15 +105,9 @@
     <t>Uniformisation des balises XML avec le client</t>
   </si>
   <si>
-    <t>Faire le tableau Excel et le détail des tâches du Sprint 6</t>
-  </si>
-  <si>
     <t>Point intermédiaire</t>
   </si>
   <si>
-    <t>Tâches terminé le 02/04/2024</t>
-  </si>
-  <si>
     <t>Tâche terminé le 02/04/2024</t>
   </si>
   <si>
@@ -124,6 +118,15 @@
   </si>
   <si>
     <t>Faire un rapport sur l'ensemble du projet</t>
+  </si>
+  <si>
+    <t>(Poursuivit dans la deuxième partie du Sprint 6)</t>
+  </si>
+  <si>
+    <t>Amélioration des fichiers références avec le client</t>
+  </si>
+  <si>
+    <t>Faire le tableau Excel et le détail des tâches du Sprint 6 - Partie 1</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,12 +173,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,22 +207,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25C790B-9A69-420E-ADEC-218324962F86}">
-  <dimension ref="A1:AD21"/>
+  <dimension ref="A1:AD20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +573,7 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -589,7 +585,7 @@
       <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -598,10 +594,10 @@
       <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="10" t="s">
+      <c r="P1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -640,7 +636,7 @@
       <c r="AC1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AD1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -861,7 +857,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5">
@@ -1085,33 +1081,27 @@
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="A16" s="10"/>
       <c r="B16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
+      <c r="A17" s="8"/>
       <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1123,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA30D50F-0BD7-4D6D-98EF-6C8A8DFFE157}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1136,84 +1126,110 @@
     <col min="3" max="3" width="40.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
-        <f>B4+B7+B8+B10+B11+B12+B13</f>
-        <v>7</v>
+      <c r="B16">
+        <f>B4+B7+B8+B9+B11+B12+B13+B14</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>